<commit_message>
working downloads for all three apps
</commit_message>
<xml_diff>
--- a/inst/app/www/Titelblatt.xlsx
+++ b/inst/app/www/Titelblatt.xlsx
@@ -1,27 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\Projekte\Bodenpreise\6_Shiny\LIMA_2.0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sszmea\R\lima-golem\inst\app\www\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DEDA07F-9D11-49B9-88E2-53389E45821C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15300" windowHeight="7245"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
     <sheet name="Erläuterungen F1" sheetId="3" r:id="rId2"/>
     <sheet name="Erläuterungen F2" sheetId="4" r:id="rId3"/>
+    <sheet name="Erläuterungen F3" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="81">
   <si>
     <t>Napfgasse 6, 8022 Zürich</t>
   </si>
@@ -229,12 +231,54 @@
   <si>
     <t>Preis pro Quadratmeter Wohnungsfläche bei Stockwerkeigentumskäufen</t>
   </si>
+  <si>
+    <t>EFH</t>
+  </si>
+  <si>
+    <t>MFH</t>
+  </si>
+  <si>
+    <t>WHG</t>
+  </si>
+  <si>
+    <t>UWH</t>
+  </si>
+  <si>
+    <t>NB</t>
+  </si>
+  <si>
+    <t>IGZ</t>
+  </si>
+  <si>
+    <t>UG</t>
+  </si>
+  <si>
+    <t>Bauten in übrigen Zonen</t>
+  </si>
+  <si>
+    <t>Bauten in Industrie- und Gewerbezone</t>
+  </si>
+  <si>
+    <t>Nutzbauten in Wohn- und Mischzonen</t>
+  </si>
+  <si>
+    <t>Übrige Wohnhäuser</t>
+  </si>
+  <si>
+    <t>Wohnhäuser mit Geschäftsräumen</t>
+  </si>
+  <si>
+    <t>Mehrfamilienhäuser</t>
+  </si>
+  <si>
+    <t>Einfamilienhäuser</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="13" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -310,6 +354,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="9"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -340,7 +392,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -374,12 +426,13 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="3" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
-    <cellStyle name="Standard 2" xfId="1"/>
-    <cellStyle name="Standard 2 2" xfId="2"/>
-    <cellStyle name="Standard 3" xfId="3"/>
+    <cellStyle name="Standard 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Standard 2 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Standard 3" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -620,10 +673,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
@@ -697,11 +750,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A5" sqref="A5:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -745,26 +798,26 @@
     </row>
     <row r="5" spans="1:2" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -862,11 +915,161 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:B17"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="27.625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="70.625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="11" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="3" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="8"/>
+      <c r="B16" s="5"/>
+    </row>
+    <row r="17" spans="1:2" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="8"/>
+      <c r="B17" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <headerFooter scaleWithDoc="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65394643-FD56-433D-BBD4-FCFB3A67E6F0}">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -885,7 +1088,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="13" t="s">
         <v>16</v>
       </c>
       <c r="B2" s="12" t="s">
@@ -893,7 +1096,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="13" t="s">
         <v>18</v>
       </c>
       <c r="B3" s="12" t="s">
@@ -901,7 +1104,7 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="13" t="s">
         <v>20</v>
       </c>
       <c r="B4" s="12" t="s">
@@ -909,7 +1112,7 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="13" t="s">
         <v>51</v>
       </c>
       <c r="B5" s="12" t="s">
@@ -917,7 +1120,7 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="13" t="s">
         <v>28</v>
       </c>
       <c r="B6" s="12" t="s">
@@ -925,7 +1128,7 @@
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="13" t="s">
         <v>30</v>
       </c>
       <c r="B7" s="12" t="s">
@@ -933,7 +1136,7 @@
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="13" t="s">
         <v>53</v>
       </c>
       <c r="B8" s="12" t="s">
@@ -941,7 +1144,7 @@
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="13" t="s">
         <v>55</v>
       </c>
       <c r="B9" s="12" t="s">
@@ -949,7 +1152,7 @@
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="13" t="s">
         <v>57</v>
       </c>
       <c r="B10" s="12" t="s">
@@ -957,7 +1160,7 @@
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="12" t="s">
+      <c r="A11" s="13" t="s">
         <v>59</v>
       </c>
       <c r="B11" s="12" t="s">
@@ -965,7 +1168,7 @@
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="12" t="s">
+      <c r="A12" s="13" t="s">
         <v>61</v>
       </c>
       <c r="B12" s="12" t="s">
@@ -973,7 +1176,7 @@
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="12" t="s">
+      <c r="A13" s="13" t="s">
         <v>63</v>
       </c>
       <c r="B13" s="12" t="s">
@@ -981,7 +1184,7 @@
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="12" t="s">
+      <c r="A14" s="13" t="s">
         <v>65</v>
       </c>
       <c r="B14" s="12" t="s">

</xml_diff>